<commit_message>
AE-5 Estudar o modelo de dados definido para a RSL
</commit_message>
<xml_diff>
--- a/sprints_formatadas.xlsx
+++ b/sprints_formatadas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,42 +527,42 @@
         <v>45672</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
         <v>14</v>
       </c>
       <c r="F2" t="n">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G2" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H2" t="n">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="I2" t="n">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Mobile</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>2.7</v>
+        <v>4.1</v>
       </c>
       <c r="L2" t="n">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="M2" t="n">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="N2" t="n">
-        <v>44.08</v>
+        <v>66.98</v>
       </c>
       <c r="O2" t="n">
-        <v>21.5</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="3">
@@ -578,22 +578,22 @@
         <v>45686</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
         <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G3" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H3" t="n">
-        <v>130</v>
+        <v>76</v>
       </c>
       <c r="I3" t="n">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -601,19 +601,19 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>3.9</v>
+        <v>2.6</v>
       </c>
       <c r="L3" t="n">
-        <v>0.17</v>
+        <v>0.1</v>
       </c>
       <c r="M3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="N3" t="n">
-        <v>67.23</v>
+        <v>34.02</v>
       </c>
       <c r="O3" t="n">
-        <v>32.5</v>
+        <v>25.33</v>
       </c>
     </row>
     <row r="4">
@@ -629,42 +629,42 @@
         <v>45700</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
         <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="G4" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="H4" t="n">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="I4" t="n">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Dados</t>
+          <t>Mobile</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="L4" t="n">
-        <v>0.24</v>
+        <v>0.19</v>
       </c>
       <c r="M4" t="n">
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
       <c r="N4" t="n">
-        <v>50.18</v>
+        <v>68.04000000000001</v>
       </c>
       <c r="O4" t="n">
-        <v>19.25</v>
+        <v>12.29</v>
       </c>
     </row>
     <row r="5">
@@ -680,22 +680,22 @@
         <v>45714</v>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E5" t="n">
         <v>14</v>
       </c>
       <c r="F5" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G5" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H5" t="n">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="I5" t="n">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -703,19 +703,19 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>3.6</v>
+        <v>4.1</v>
       </c>
       <c r="L5" t="n">
-        <v>0.14</v>
+        <v>0.19</v>
       </c>
       <c r="M5" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="N5" t="n">
-        <v>43.96</v>
+        <v>56.08</v>
       </c>
       <c r="O5" t="n">
-        <v>31.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="6">
@@ -731,42 +731,297 @@
         <v>45728</v>
       </c>
       <c r="D6" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E6" t="n">
         <v>14</v>
       </c>
       <c r="F6" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="G6" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H6" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I6" t="n">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
+          <t>Dados</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="N6" t="n">
+        <v>33.97</v>
+      </c>
+      <c r="O6" t="n">
+        <v>13.14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sprint_06</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>45728</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>45742</v>
+      </c>
+      <c r="D7" t="n">
+        <v>7</v>
+      </c>
+      <c r="E7" t="n">
+        <v>14</v>
+      </c>
+      <c r="F7" t="n">
+        <v>44</v>
+      </c>
+      <c r="G7" t="n">
+        <v>34</v>
+      </c>
+      <c r="H7" t="n">
+        <v>109</v>
+      </c>
+      <c r="I7" t="n">
+        <v>104</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Dados</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>3</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="N7" t="n">
+        <v>56.34</v>
+      </c>
+      <c r="O7" t="n">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sprint_07</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>45742</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>45756</v>
+      </c>
+      <c r="D8" t="n">
+        <v>7</v>
+      </c>
+      <c r="E8" t="n">
+        <v>14</v>
+      </c>
+      <c r="F8" t="n">
+        <v>29</v>
+      </c>
+      <c r="G8" t="n">
+        <v>28</v>
+      </c>
+      <c r="H8" t="n">
+        <v>104</v>
+      </c>
+      <c r="I8" t="n">
+        <v>102</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
           <t>Mobile</t>
         </is>
       </c>
-      <c r="K6" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="N6" t="n">
-        <v>59.11</v>
-      </c>
-      <c r="O6" t="n">
-        <v>18.6</v>
+      <c r="K8" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N8" t="n">
+        <v>45.68</v>
+      </c>
+      <c r="O8" t="n">
+        <v>14.86</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Sprint_08</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>45756</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>45770</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" t="n">
+        <v>14</v>
+      </c>
+      <c r="F9" t="n">
+        <v>45</v>
+      </c>
+      <c r="G9" t="n">
+        <v>41</v>
+      </c>
+      <c r="H9" t="n">
+        <v>83</v>
+      </c>
+      <c r="I9" t="n">
+        <v>77</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Dados</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="N9" t="n">
+        <v>62.75</v>
+      </c>
+      <c r="O9" t="n">
+        <v>13.83</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Sprint_09</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>45770</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>14</v>
+      </c>
+      <c r="F10" t="n">
+        <v>28</v>
+      </c>
+      <c r="G10" t="n">
+        <v>23</v>
+      </c>
+      <c r="H10" t="n">
+        <v>95</v>
+      </c>
+      <c r="I10" t="n">
+        <v>70</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>API</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="N10" t="n">
+        <v>64.04000000000001</v>
+      </c>
+      <c r="O10" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sprint_10</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>45784</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>45798</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" t="n">
+        <v>14</v>
+      </c>
+      <c r="F11" t="n">
+        <v>50</v>
+      </c>
+      <c r="G11" t="n">
+        <v>46</v>
+      </c>
+      <c r="H11" t="n">
+        <v>65</v>
+      </c>
+      <c r="I11" t="n">
+        <v>53</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Dados</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="N11" t="n">
+        <v>48.75</v>
+      </c>
+      <c r="O11" t="n">
+        <v>16.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>